<commit_message>
Update sheets with new information and added comments
</commit_message>
<xml_diff>
--- a/Raw/TastingAnalysis.xlsx
+++ b/Raw/TastingAnalysis.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17766"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daniel\Dropbox\Asana\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeffrey\Desktop\Paradyme\Catering\Raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="TastingAnalysis" sheetId="3" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -129,7 +129,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
@@ -610,8 +610,6 @@
     <xf numFmtId="165" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="165" fontId="4" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -628,6 +626,8 @@
     </xf>
     <xf numFmtId="3" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -646,7 +646,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -740,7 +740,7 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000004-2D67-4DA1-BD07-ADF1D46769C2}"/>
               </c:ext>
@@ -764,7 +764,7 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000005-2D67-4DA1-BD07-ADF1D46769C2}"/>
               </c:ext>
@@ -788,7 +788,7 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000003-2D67-4DA1-BD07-ADF1D46769C2}"/>
               </c:ext>
@@ -810,11 +810,11 @@
               <c:showSerName val="0"/>
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000003-2D67-4DA1-BD07-ADF1D46769C2}"/>
                 </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -883,7 +883,7 @@
                 <a:effectLst/>
               </c:spPr>
             </c:leaderLines>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
@@ -922,7 +922,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-2D67-4DA1-BD07-ADF1D46769C2}"/>
             </c:ext>
@@ -1038,7 +1038,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1149,7 +1149,7 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000001-7198-40AD-9DE1-E75D896FA3F5}"/>
               </c:ext>
@@ -1173,7 +1173,7 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000003-7198-40AD-9DE1-E75D896FA3F5}"/>
               </c:ext>
@@ -1197,7 +1197,7 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000005-7198-40AD-9DE1-E75D896FA3F5}"/>
               </c:ext>
@@ -1219,11 +1219,11 @@
               <c:showSerName val="0"/>
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000005-7198-40AD-9DE1-E75D896FA3F5}"/>
                 </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -1292,7 +1292,7 @@
                 <a:effectLst/>
               </c:spPr>
             </c:leaderLines>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
@@ -1331,7 +1331,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000006-7198-40AD-9DE1-E75D896FA3F5}"/>
             </c:ext>
@@ -1411,7 +1411,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1505,7 +1505,7 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000001-90FA-4830-A8A4-546B4699F8CC}"/>
               </c:ext>
@@ -1529,7 +1529,7 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000003-90FA-4830-A8A4-546B4699F8CC}"/>
               </c:ext>
@@ -1553,7 +1553,7 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000005-90FA-4830-A8A4-546B4699F8CC}"/>
               </c:ext>
@@ -1575,11 +1575,11 @@
               <c:showSerName val="0"/>
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000005-90FA-4830-A8A4-546B4699F8CC}"/>
                 </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -1648,7 +1648,7 @@
                 <a:effectLst/>
               </c:spPr>
             </c:leaderLines>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
@@ -1684,7 +1684,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000006-90FA-4830-A8A4-546B4699F8CC}"/>
             </c:ext>
@@ -3706,7 +3706,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2412819E-E177-41D4-A33B-A728E74402FF}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2412819E-E177-41D4-A33B-A728E74402FF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3742,7 +3742,7 @@
         <xdr:cNvPr id="6" name="Chart 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B27E976-5132-460F-BD27-7C4527D104A7}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B27E976-5132-460F-BD27-7C4527D104A7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3780,7 +3780,7 @@
         <xdr:cNvPr id="7" name="Chart 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{17A7E582-7EC4-47E6-A65D-884AA9832FC0}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{17A7E582-7EC4-47E6-A65D-884AA9832FC0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3879,23 +3879,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -3931,23 +3914,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -4127,8 +4093,8 @@
   <dimension ref="A2:R64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E42" sqref="E42"/>
+      <pane ySplit="4" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4147,15 +4113,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="62" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C3" s="6" t="s">
@@ -4683,11 +4649,11 @@
         <v>0</v>
       </c>
       <c r="N13" s="11">
-        <f t="shared" ref="N13:N27" si="4">K13/(G13+D13)</f>
+        <f t="shared" ref="N13:N28" si="4">K13/(G13+D13)</f>
         <v>18602.206896551725</v>
       </c>
       <c r="O13" s="11">
-        <f t="shared" ref="O13:O27" si="5">L13/H13</f>
+        <f t="shared" ref="O13:O28" si="5">L13/H13</f>
         <v>14421.8</v>
       </c>
       <c r="P13" s="18"/>
@@ -5406,23 +5372,50 @@
       <c r="B28" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="C28" s="33"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="34"/>
-      <c r="F28" s="33"/>
-      <c r="G28" s="21"/>
-      <c r="H28" s="21"/>
-      <c r="I28" s="34"/>
-      <c r="J28" s="41" t="e">
+      <c r="C28" s="33">
+        <v>12</v>
+      </c>
+      <c r="D28" s="21">
+        <v>12</v>
+      </c>
+      <c r="E28" s="34">
+        <v>12</v>
+      </c>
+      <c r="F28" s="33">
+        <v>12</v>
+      </c>
+      <c r="G28" s="21">
+        <v>12</v>
+      </c>
+      <c r="H28" s="21">
+        <v>12</v>
+      </c>
+      <c r="I28" s="34">
+        <v>1</v>
+      </c>
+      <c r="J28" s="41">
         <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K28" s="8"/>
-      <c r="L28" s="8"/>
-      <c r="M28" s="18"/>
-      <c r="N28" s="8"/>
-      <c r="O28" s="8"/>
-      <c r="P28" s="18"/>
+        <v>100</v>
+      </c>
+      <c r="K28" s="8">
+        <v>111111</v>
+      </c>
+      <c r="L28" s="8">
+        <v>123123</v>
+      </c>
+      <c r="M28" s="18">
+        <v>12312</v>
+      </c>
+      <c r="N28" s="8">
+        <v>123123</v>
+      </c>
+      <c r="O28" s="8">
+        <f t="shared" si="5"/>
+        <v>10260.25</v>
+      </c>
+      <c r="P28" s="18">
+        <v>11111</v>
+      </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
@@ -5615,59 +5608,59 @@
       </c>
       <c r="C37" s="37">
         <f t="shared" ref="C37:I37" si="8">SUM(C25:C36)</f>
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="D37" s="23">
         <f t="shared" si="8"/>
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="E37" s="38">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="F37" s="37">
         <f t="shared" si="8"/>
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="G37" s="23">
         <f t="shared" si="8"/>
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="H37" s="23">
         <f t="shared" si="8"/>
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="I37" s="38">
         <f t="shared" si="8"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J37" s="45">
         <f t="shared" si="7"/>
-        <v>63.265306122448983</v>
+        <v>70.491803278688522</v>
       </c>
       <c r="K37" s="12">
         <f>SUM(K25:K36)</f>
-        <v>1026571</v>
+        <v>1137682</v>
       </c>
       <c r="L37" s="12">
         <f>SUM(L25:L36)</f>
-        <v>166271</v>
+        <v>289394</v>
       </c>
       <c r="M37" s="12">
         <f>SUM(M25:M36)</f>
-        <v>152510</v>
+        <v>164822</v>
       </c>
       <c r="N37" s="12">
         <f>AVERAGE(N25:N36)</f>
-        <v>17330.402448397013</v>
+        <v>43778.55183629776</v>
       </c>
       <c r="O37" s="12">
         <f>AVERAGE(O25:O36)</f>
-        <v>24704.2</v>
+        <v>21093.212500000001</v>
       </c>
       <c r="P37" s="13">
         <f>AVERAGE(P25:P36)</f>
-        <v>16812.958333333332</v>
+        <v>14912.305555555555</v>
       </c>
     </row>
     <row r="38" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5678,14 +5671,14 @@
         <f>G24/F24</f>
         <v>0.74371859296482412</v>
       </c>
-      <c r="K38" s="61" t="s">
+      <c r="K38" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="L38" s="62"/>
-      <c r="M38" s="62"/>
-      <c r="N38" s="62"/>
-      <c r="O38" s="62"/>
-      <c r="P38" s="63"/>
+      <c r="L38" s="60"/>
+      <c r="M38" s="60"/>
+      <c r="N38" s="60"/>
+      <c r="O38" s="60"/>
+      <c r="P38" s="61"/>
       <c r="Q38" s="50"/>
       <c r="R38" s="50"/>
     </row>
@@ -5695,48 +5688,48 @@
       <c r="F39"/>
       <c r="J39" s="49">
         <f>G37/F37</f>
-        <v>0.63265306122448983</v>
-      </c>
-      <c r="K39" s="61" t="s">
+        <v>0.70491803278688525</v>
+      </c>
+      <c r="K39" s="59" t="s">
         <v>30</v>
       </c>
-      <c r="L39" s="59"/>
-      <c r="M39" s="59"/>
-      <c r="N39" s="59"/>
-      <c r="O39" s="59"/>
-      <c r="P39" s="59"/>
+      <c r="L39" s="57"/>
+      <c r="M39" s="57"/>
+      <c r="N39" s="57"/>
+      <c r="O39" s="57"/>
+      <c r="P39" s="57"/>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D40"/>
       <c r="E40"/>
       <c r="F40">
         <f>SUM(F25:F36)</f>
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="G40">
         <f>SUM(G25:G36)</f>
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="H40">
         <f>SUM(H25:H36)</f>
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="I40">
         <f>SUM(I25:I36)</f>
-        <v>10</v>
-      </c>
-      <c r="J40" s="54">
+        <v>11</v>
+      </c>
+      <c r="J40" s="52">
         <f>G40/(G40+H40)</f>
-        <v>0.79487179487179482</v>
-      </c>
-      <c r="K40" s="55" t="s">
+        <v>0.68253968253968256</v>
+      </c>
+      <c r="K40" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="L40" s="56"/>
-      <c r="M40" s="56"/>
-      <c r="N40" s="56"/>
-      <c r="O40" s="56"/>
-      <c r="P40" s="56"/>
+      <c r="L40" s="54"/>
+      <c r="M40" s="54"/>
+      <c r="N40" s="54"/>
+      <c r="O40" s="54"/>
+      <c r="P40" s="54"/>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D41"/>
@@ -5757,18 +5750,18 @@
         <f>I25+I26+I27</f>
         <v>10</v>
       </c>
-      <c r="J41" s="57">
+      <c r="J41" s="55">
         <f>G41/F41</f>
         <v>0.63265306122448983</v>
       </c>
-      <c r="K41" s="58" t="s">
+      <c r="K41" s="56" t="s">
         <v>28</v>
       </c>
-      <c r="L41" s="59"/>
-      <c r="M41" s="59"/>
-      <c r="N41" s="59"/>
-      <c r="O41" s="59"/>
-      <c r="P41" s="59"/>
+      <c r="L41" s="57"/>
+      <c r="M41" s="57"/>
+      <c r="N41" s="57"/>
+      <c r="O41" s="57"/>
+      <c r="P41" s="57"/>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D42"/>
@@ -5785,18 +5778,18 @@
         <f>F42-G42</f>
         <v>10.560000000000002</v>
       </c>
-      <c r="J42" s="60">
+      <c r="J42" s="58">
         <f>G42/F42</f>
         <v>0.78448979591836732</v>
       </c>
-      <c r="K42" s="55" t="s">
+      <c r="K42" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="L42" s="56"/>
-      <c r="M42" s="56"/>
-      <c r="N42" s="56"/>
-      <c r="O42" s="56"/>
-      <c r="P42" s="56"/>
+      <c r="L42" s="54"/>
+      <c r="M42" s="54"/>
+      <c r="N42" s="54"/>
+      <c r="O42" s="54"/>
+      <c r="P42" s="54"/>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="K43" s="46"/>
@@ -5883,8 +5876,8 @@
       <c r="J50" s="48"/>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A62" s="53"/>
-      <c r="B62" s="53"/>
+      <c r="A62" s="63"/>
+      <c r="B62" s="63"/>
       <c r="C62" s="46"/>
       <c r="D62" s="46"/>
       <c r="E62" s="46"/>
@@ -5893,8 +5886,8 @@
       <c r="H62" s="46"/>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A63" s="53"/>
-      <c r="B63" s="53"/>
+      <c r="A63" s="63"/>
+      <c r="B63" s="63"/>
       <c r="C63" s="46"/>
       <c r="D63" s="48"/>
       <c r="E63" s="48"/>

</xml_diff>